<commit_message>
issue #6: Datatypes correction incl. tests
</commit_message>
<xml_diff>
--- a/test/type_test_data.xlsx
+++ b/test/type_test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d3f1d7ac472c409/Documents/Projekts/SCOUT/Pyadomd/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{BA22AA32-E09E-4DB0-A1A2-0FA9D71CBE0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4B4274F3-1552-4B15-9554-23AD34E2D2A7}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{BA22AA32-E09E-4DB0-A1A2-0FA9D71CBE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7998BA61-DB0B-4D09-ADD7-BDBC45E11E21}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E76436C8-3FDA-4380-AC69-487EAE89CB13}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Integer</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
   </si>
 </sst>
 </file>
@@ -167,8 +173,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B52855C7-67BB-47CF-9765-0619DCC35105}" name="Table1" displayName="Table1" ref="A1:F3" totalsRowShown="0">
-  <autoFilter ref="A1:F3" xr:uid="{568CD807-F7A2-4F29-B919-C7E81486C69E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B52855C7-67BB-47CF-9765-0619DCC35105}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{568CD807-F7A2-4F29-B919-C7E81486C69E}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1235BF2E-0171-4587-9545-B02AAD386CAF}" name="String"/>
     <tableColumn id="2" xr3:uid="{291DB26C-17FE-4AF0-B577-0804CC2B1DC9}" name="Integer"/>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C812405-BFC1-4318-86FB-E46C5AAD7382}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,11 +539,36 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>+""</f>
-        <v/>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44196</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44196</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>